<commit_message>
SAJE and GIAD BRIEF results added
</commit_message>
<xml_diff>
--- a/data/LELI_brief.xlsx
+++ b/data/LELI_brief.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/aaron_pilot_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93795CC1-2414-384C-8171-4DA30DFFC00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F439C6C9-E2DA-7F4C-BCAD-54658DC57C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15660" xr2:uid="{11F1717A-72AE-CB42-AE29-0C1B97B79501}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B2" sqref="B2:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,204 +472,60 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>39</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>39</v>
-      </c>
-      <c r="E2">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>49</v>
-      </c>
-      <c r="C3">
-        <v>65</v>
-      </c>
-      <c r="D3">
-        <v>58</v>
-      </c>
-      <c r="E3">
-        <v>84</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>53</v>
-      </c>
-      <c r="C4">
-        <v>74</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>66</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>42</v>
-      </c>
-      <c r="C5">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>38</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>45</v>
-      </c>
-      <c r="C6">
-        <v>46</v>
-      </c>
-      <c r="D6">
-        <v>42</v>
-      </c>
-      <c r="E6">
-        <v>28</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>45</v>
-      </c>
-      <c r="C7">
-        <v>53</v>
-      </c>
-      <c r="D7">
-        <v>42</v>
-      </c>
-      <c r="E7">
-        <v>35</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>40</v>
-      </c>
-      <c r="C8">
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <v>40</v>
-      </c>
-      <c r="E8">
-        <v>26</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>45</v>
-      </c>
-      <c r="C9">
-        <v>48</v>
-      </c>
-      <c r="D9">
-        <v>42</v>
-      </c>
-      <c r="E9">
-        <v>38</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>38</v>
-      </c>
-      <c r="C10">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>38</v>
-      </c>
-      <c r="E10">
-        <v>16</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>44</v>
-      </c>
-      <c r="C11">
-        <v>36</v>
-      </c>
-      <c r="D11">
-        <v>38</v>
-      </c>
-      <c r="E11">
-        <v>17</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>39</v>
-      </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>36</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
-      </c>
-      <c r="B13">
-        <v>41</v>
-      </c>
-      <c r="C13">
-        <v>18</v>
-      </c>
-      <c r="D13">
-        <v>37</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>